<commit_message>
Add .gitignore file and update FIS Prework.
</commit_message>
<xml_diff>
--- a/FIS_Prework_WebDev.xlsx
+++ b/FIS_Prework_WebDev.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="FIS PreWork - Web Dev" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>The Flatiron School Prework</t>
   </si>
@@ -36,12 +36,6 @@
     <t>Date Done</t>
   </si>
   <si>
-    <t>Web Dev</t>
-  </si>
-  <si>
-    <t>Full Class</t>
-  </si>
-  <si>
     <t>Website Basics</t>
   </si>
   <si>
@@ -54,24 +48,6 @@
     <t>HTML</t>
   </si>
   <si>
-    <t>Command Line Tutorial</t>
-  </si>
-  <si>
-    <t>Getting Started with the Console</t>
-  </si>
-  <si>
-    <t>Environment and Redirection</t>
-  </si>
-  <si>
-    <t>Console Foundations</t>
-  </si>
-  <si>
-    <t>Learn the Cmd Line the Hard Way</t>
-  </si>
-  <si>
-    <t>Command Line Basics</t>
-  </si>
-  <si>
     <t>CSS</t>
   </si>
   <si>
@@ -81,31 +57,10 @@
     <t>Treehouse HTML Basics</t>
   </si>
   <si>
-    <t>Advanced HTML5 &amp; CSS</t>
-  </si>
-  <si>
-    <t>JavaScript</t>
-  </si>
-  <si>
     <t>CSS Foundations</t>
   </si>
   <si>
     <t>CSS Cross Country</t>
-  </si>
-  <si>
-    <t>Reponsive Websites</t>
-  </si>
-  <si>
-    <t>Programming</t>
-  </si>
-  <si>
-    <t>Basics</t>
-  </si>
-  <si>
-    <t>Try Ruby</t>
-  </si>
-  <si>
-    <t>Introduction to Programming</t>
   </si>
   <si>
     <t>Javascript</t>
@@ -165,13 +120,31 @@
   </si>
   <si>
     <t>Rails Best Practices</t>
+  </si>
+  <si>
+    <t>Aesthetics</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Build HTML / CSS Website from Scratch</t>
+  </si>
+  <si>
+    <t>Websites</t>
+  </si>
+  <si>
+    <t>Functional HTML &amp; CSS3</t>
+  </si>
+  <si>
+    <t>Build a Responsive Website</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,6 +173,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -285,7 +266,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -510,19 +491,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="double">
-        <color auto="1"/>
-      </top>
-      <bottom style="dashed">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -546,32 +514,6 @@
         <color auto="1"/>
       </top>
       <bottom style="dashed">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="dashed">
-        <color auto="1"/>
-      </top>
-      <bottom style="dashed">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="dashed">
-        <color auto="1"/>
-      </top>
-      <bottom style="double">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -736,15 +678,146 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -752,187 +825,36 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="10" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="10" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="10" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="10" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1263,10 +1185,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E45"/>
+  <dimension ref="B1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1281,363 +1203,306 @@
   <sheetData>
     <row r="1" spans="2:5" ht="18.75" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="47"/>
     </row>
     <row r="3" spans="2:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1"/>
     <row r="4" spans="2:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="E5" s="4">
+        <v>41368</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B6" s="49"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="E6" s="6">
+        <v>41368</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
+      <c r="B7" s="49"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="9">
-        <v>41368</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B6" s="10"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="11" t="s">
+      <c r="E7" s="4">
+        <v>41373</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B8" s="49"/>
+      <c r="C8" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
+      <c r="B9" s="49"/>
+      <c r="C9" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="12">
-        <v>41368</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B7" s="10"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="13" t="s">
+      <c r="D9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="9">
+        <v>41421</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B10" s="49"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="6">
+        <v>41422</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B11" s="49"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="6">
+        <v>41422</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B12" s="49"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B13" s="49"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
+      <c r="B14" s="49"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="11"/>
+    </row>
+    <row r="15" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
+      <c r="B15" s="49"/>
+      <c r="C15" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="9">
-        <v>41373</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B8" s="10"/>
-      <c r="C8" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="16">
-        <v>41421</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B9" s="10"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="11" t="s">
+      <c r="D15" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="12"/>
-    </row>
-    <row r="10" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B10" s="10"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="11" t="s">
+      <c r="E15" s="9"/>
+    </row>
+    <row r="16" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B16" s="49"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="12"/>
-    </row>
-    <row r="11" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B11" s="10"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="11" t="s">
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
+      <c r="B17" s="49"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="11"/>
+    </row>
+    <row r="18" spans="2:5" ht="3.75" customHeight="1" thickTop="1">
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="15"/>
+    </row>
+    <row r="19" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B19" s="37"/>
+      <c r="C19" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="12"/>
-    </row>
-    <row r="12" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B12" s="10"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="11" t="s">
+      <c r="D19" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="12">
-        <v>41421</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B13" s="10"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="19" t="s">
+      <c r="E19" s="24">
+        <v>41425</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B20" s="37"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="20"/>
-    </row>
-    <row r="14" spans="2:5" s="1" customFormat="1" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B14" s="10"/>
-      <c r="C14" s="14" t="s">
+      <c r="E20" s="55"/>
+    </row>
+    <row r="21" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
+      <c r="B21" s="37"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="E21" s="22"/>
+    </row>
+    <row r="22" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
+      <c r="B22" s="37"/>
+      <c r="C22" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="16">
-        <v>41421</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" s="1" customFormat="1" ht="18.75" customHeight="1">
-      <c r="B15" s="10"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="11" t="s">
+      <c r="D22" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="12">
-        <v>41422</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" s="1" customFormat="1" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B16" s="10"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="19" t="s">
+      <c r="E22" s="23"/>
+    </row>
+    <row r="23" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B23" s="37"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="20">
-        <v>41422</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" s="1" customFormat="1" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B17" s="10"/>
-      <c r="C17" s="21" t="s">
+      <c r="E23" s="24">
+        <v>41427</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
+      <c r="B24" s="37"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="E24" s="22"/>
+    </row>
+    <row r="25" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
+      <c r="B25" s="37"/>
+      <c r="C25" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="23"/>
-    </row>
-    <row r="18" spans="2:5" s="1" customFormat="1" ht="18.75" customHeight="1">
-      <c r="B18" s="10"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="11" t="s">
+      <c r="D25" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="25"/>
-    </row>
-    <row r="19" spans="2:5" s="1" customFormat="1" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B19" s="10"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="27" t="s">
+      <c r="E25" s="20"/>
+    </row>
+    <row r="26" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B26" s="37"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="28"/>
-    </row>
-    <row r="20" spans="2:5" s="1" customFormat="1" ht="3.75" customHeight="1" thickTop="1">
-      <c r="B20" s="29"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="32"/>
-    </row>
-    <row r="21" spans="2:5" s="1" customFormat="1" ht="18.75" customHeight="1">
-      <c r="B21" s="33" t="s">
+      <c r="E26" s="17"/>
+    </row>
+    <row r="27" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B27" s="37"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="34" t="s">
+      <c r="E27" s="24"/>
+    </row>
+    <row r="28" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B28" s="37"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="35" t="s">
+      <c r="E28" s="26"/>
+    </row>
+    <row r="29" spans="2:5" ht="3.75" customHeight="1">
+      <c r="B29" s="27"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="15"/>
+    </row>
+    <row r="30" spans="2:5" ht="26.25" customHeight="1">
+      <c r="B30" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="36">
-        <v>41423</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" s="1" customFormat="1" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B22" s="33"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="38" t="s">
+      <c r="C30" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="E22" s="39">
-        <v>41424</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" s="1" customFormat="1" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B23" s="33"/>
-      <c r="C23" s="40" t="s">
+      <c r="D30" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="41" t="s">
+      <c r="E30" s="30"/>
+    </row>
+    <row r="31" spans="2:5" ht="26.25" customHeight="1" thickBot="1">
+      <c r="B31" s="41"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="42">
-        <v>41425</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" s="1" customFormat="1" ht="18.75" customHeight="1">
-      <c r="B24" s="33"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="43" t="s">
+      <c r="E31" s="32"/>
+    </row>
+    <row r="32" spans="2:5" ht="56.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B32" s="42"/>
+      <c r="C32" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="44"/>
-    </row>
-    <row r="25" spans="2:5" s="1" customFormat="1" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B25" s="33"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="38" t="s">
+      <c r="D32" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="45"/>
-    </row>
-    <row r="26" spans="2:5" s="1" customFormat="1" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B26" s="33"/>
-      <c r="C26" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="41" t="s">
-        <v>34</v>
-      </c>
-      <c r="E26" s="46"/>
-    </row>
-    <row r="27" spans="2:5" s="1" customFormat="1" ht="18.75" customHeight="1">
-      <c r="B27" s="33"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="E27" s="47">
-        <v>41427</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" s="1" customFormat="1" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B28" s="33"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="E28" s="45"/>
-    </row>
-    <row r="29" spans="2:5" s="1" customFormat="1" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B29" s="33"/>
-      <c r="C29" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="D29" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="E29" s="42"/>
-    </row>
-    <row r="30" spans="2:5" s="1" customFormat="1" ht="18.75" customHeight="1">
-      <c r="B30" s="33"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="E30" s="36"/>
-    </row>
-    <row r="31" spans="2:5" s="1" customFormat="1" ht="18.75" customHeight="1">
-      <c r="B31" s="33"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="43" t="s">
-        <v>40</v>
-      </c>
-      <c r="E31" s="47"/>
-    </row>
-    <row r="32" spans="2:5" s="1" customFormat="1" ht="18.75" customHeight="1">
-      <c r="B32" s="33"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="48" t="s">
-        <v>41</v>
-      </c>
-      <c r="E32" s="49"/>
-    </row>
-    <row r="33" spans="2:5" s="1" customFormat="1" ht="3.75" customHeight="1">
-      <c r="B33" s="50"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="32"/>
-    </row>
-    <row r="34" spans="2:5" s="1" customFormat="1" ht="26.25" customHeight="1">
-      <c r="B34" s="52" t="s">
-        <v>42</v>
-      </c>
-      <c r="C34" s="53" t="s">
-        <v>43</v>
-      </c>
-      <c r="D34" s="54" t="s">
-        <v>44</v>
-      </c>
-      <c r="E34" s="55"/>
-    </row>
-    <row r="35" spans="2:5" s="1" customFormat="1" ht="26.25" customHeight="1" thickBot="1">
-      <c r="B35" s="52"/>
-      <c r="C35" s="56"/>
-      <c r="D35" s="57" t="s">
-        <v>45</v>
-      </c>
-      <c r="E35" s="58"/>
-    </row>
-    <row r="36" spans="2:5" s="1" customFormat="1" ht="56.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B36" s="59"/>
-      <c r="C36" s="60" t="s">
-        <v>46</v>
-      </c>
-      <c r="D36" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="E36" s="62"/>
-    </row>
-    <row r="37" spans="2:5" s="1" customFormat="1" ht="18.75" customHeight="1" thickTop="1"/>
-    <row r="38" spans="2:5" s="1" customFormat="1" ht="18.75" customHeight="1">
-      <c r="E38" s="63"/>
-    </row>
-    <row r="39" spans="2:5" s="1" customFormat="1" ht="18.75" customHeight="1">
-      <c r="E39" s="63"/>
-    </row>
-    <row r="40" spans="2:5" s="1" customFormat="1" ht="18.75" customHeight="1"/>
-    <row r="41" spans="2:5" s="1" customFormat="1" ht="18.75" customHeight="1"/>
-    <row r="42" spans="2:5" s="1" customFormat="1" ht="18.75" customHeight="1"/>
-    <row r="43" spans="2:5" s="1" customFormat="1" ht="18.75" customHeight="1"/>
-    <row r="44" spans="2:5" s="1" customFormat="1" ht="18.75" customHeight="1"/>
-    <row r="45" spans="2:5" s="1" customFormat="1" ht="18.75" customHeight="1"/>
+      <c r="E32" s="35"/>
+    </row>
+    <row r="33" spans="5:5" ht="18.75" customHeight="1" thickTop="1"/>
+    <row r="34" spans="5:5" ht="18.75" customHeight="1">
+      <c r="E34" s="36"/>
+    </row>
+    <row r="35" spans="5:5" ht="18.75" customHeight="1">
+      <c r="E35" s="36"/>
+    </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="B21:B32"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="C29:C32"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="C34:C35"/>
+  <mergeCells count="11">
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="C30:C31"/>
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B5:B19"/>
+    <mergeCell ref="B5:B17"/>
     <mergeCell ref="C5:C7"/>
-    <mergeCell ref="C8:C13"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="C9:C14"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="B19:B28"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="C25:C28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2:E2" r:id="rId1" display="The Flatiron School Prework"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Complete update on FIS WebDev prework.
</commit_message>
<xml_diff>
--- a/FIS_Prework_WebDev.xlsx
+++ b/FIS_Prework_WebDev.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="13400" yWindow="0" windowWidth="15400" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="FIS PreWork - Web Dev" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>The Flatiron School Prework</t>
   </si>
@@ -57,71 +57,21 @@
     <t>Treehouse HTML Basics</t>
   </si>
   <si>
+    <t>JavaScript</t>
+  </si>
+  <si>
     <t>CSS Foundations</t>
   </si>
   <si>
     <t>CSS Cross Country</t>
   </si>
   <si>
-    <t>Javascript</t>
+    <t>Programming</t>
   </si>
   <si>
     <t>Javascript Foundations</t>
   </si>
   <si>
-    <t>jQuery Air, First Flight</t>
-  </si>
-  <si>
-    <t>jQuery Air, Captain's Log</t>
-  </si>
-  <si>
-    <t>Ruby</t>
-  </si>
-  <si>
-    <t>Learn to Program</t>
-  </si>
-  <si>
-    <t>Ruby Foundations</t>
-  </si>
-  <si>
-    <t>Ruby Bits</t>
-  </si>
-  <si>
-    <t>Rails</t>
-  </si>
-  <si>
-    <t>Getting Started with Rails</t>
-  </si>
-  <si>
-    <t>Rails for Zombies (Redux)</t>
-  </si>
-  <si>
-    <t>Rails for Zombies 2</t>
-  </si>
-  <si>
-    <t>Building Facebook</t>
-  </si>
-  <si>
-    <t>Advanced
-Topics</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>Testing with Rspec</t>
-  </si>
-  <si>
-    <t>Rails Testing for Zombies</t>
-  </si>
-  <si>
-    <t>Best
-Practices</t>
-  </si>
-  <si>
-    <t>Rails Best Practices</t>
-  </si>
-  <si>
     <t>Aesthetics</t>
   </si>
   <si>
@@ -131,20 +81,38 @@
     <t>Build HTML / CSS Website from Scratch</t>
   </si>
   <si>
-    <t>Websites</t>
-  </si>
-  <si>
     <t>Functional HTML &amp; CSS3</t>
   </si>
   <si>
     <t>Build a Responsive Website</t>
+  </si>
+  <si>
+    <t>Code School HTML / CSS Track</t>
+  </si>
+  <si>
+    <t>Code School JavaScript Track</t>
+  </si>
+  <si>
+    <t>WEBSITE BASICS</t>
+  </si>
+  <si>
+    <t>JavaScript Road Trip Part 1</t>
+  </si>
+  <si>
+    <t>JavaScript Road Trip Part 2</t>
+  </si>
+  <si>
+    <t>Try jQuery</t>
+  </si>
+  <si>
+    <t>jQuery: The Return Flight</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,8 +153,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -247,26 +222,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="34">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -491,15 +448,24 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="double">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom style="dashed">
         <color auto="1"/>
       </bottom>
@@ -510,27 +476,23 @@
       <right style="thick">
         <color auto="1"/>
       </right>
-      <top style="double">
+      <top/>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
         <color auto="1"/>
       </top>
-      <bottom style="dashed">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="dashed">
-        <color auto="1"/>
-      </top>
-      <bottom style="double">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -541,150 +503,24 @@
       <top style="dashed">
         <color auto="1"/>
       </top>
-      <bottom style="double">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="dashed">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="dashed">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="double">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="double">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="dashed">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="dashed">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -719,104 +555,35 @@
     <xf numFmtId="14" fontId="0" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="10" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="10" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="10" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -826,12 +593,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -845,16 +606,35 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1185,10 +965,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E35"/>
+  <dimension ref="B1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1203,12 +983,12 @@
   <sheetData>
     <row r="1" spans="2:5" ht="18.75" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="47"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="24"/>
     </row>
     <row r="3" spans="2:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1"/>
     <row r="4" spans="2:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
@@ -1226,11 +1006,11 @@
       </c>
     </row>
     <row r="5" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B5" s="48" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="50" t="s">
-        <v>33</v>
+      <c r="B5" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>17</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>5</v>
@@ -1240,8 +1020,8 @@
       </c>
     </row>
     <row r="6" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B6" s="49"/>
-      <c r="C6" s="50"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="25"/>
       <c r="D6" s="5" t="s">
         <v>6</v>
       </c>
@@ -1250,8 +1030,8 @@
       </c>
     </row>
     <row r="7" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B7" s="49"/>
-      <c r="C7" s="50"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="25"/>
       <c r="D7" s="7" t="s">
         <v>7</v>
       </c>
@@ -1260,243 +1040,162 @@
       </c>
     </row>
     <row r="8" spans="2:5" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B8" s="49"/>
-      <c r="C8" s="54" t="s">
-        <v>34</v>
+      <c r="B8" s="34"/>
+      <c r="C8" s="17" t="s">
+        <v>18</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E8" s="9"/>
     </row>
     <row r="9" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B9" s="49"/>
-      <c r="C9" s="51" t="s">
+      <c r="B9" s="34"/>
+      <c r="C9" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B10" s="34"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E10" s="6">
         <v>41421</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B10" s="49"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="5" t="s">
+    <row r="11" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B11" s="34"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="E10" s="6">
-        <v>41422</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B11" s="49"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="E11" s="6">
         <v>41422</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B12" s="49"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B13" s="49"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B14" s="49"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="11"/>
-    </row>
-    <row r="15" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B15" s="49"/>
-      <c r="C15" s="51" t="s">
+    <row r="12" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
+      <c r="B12" s="34"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="11">
+        <v>41422</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
+      <c r="B13" s="34"/>
+      <c r="C13" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B14" s="34"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B15" s="34"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="2:5" ht="3.75" customHeight="1">
+      <c r="B16" s="19"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="13"/>
+    </row>
+    <row r="17" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B17" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="9"/>
-    </row>
-    <row r="16" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B16" s="49"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B17" s="49"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="11"/>
-    </row>
-    <row r="18" spans="2:5" ht="3.75" customHeight="1" thickTop="1">
-      <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="15"/>
+      <c r="D17" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="14"/>
+    </row>
+    <row r="18" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B18" s="32"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="21">
+        <v>41425</v>
+      </c>
     </row>
     <row r="19" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B19" s="37"/>
-      <c r="C19" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="24">
-        <v>41425</v>
-      </c>
+      <c r="B19" s="32"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="18"/>
     </row>
     <row r="20" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B20" s="37"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="55"/>
-    </row>
-    <row r="21" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B21" s="37"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" s="22"/>
-    </row>
-    <row r="22" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B22" s="37"/>
-      <c r="C22" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="23"/>
-    </row>
-    <row r="23" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B23" s="37"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" s="24">
-        <v>41427</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B24" s="37"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" s="22"/>
-    </row>
-    <row r="25" spans="2:5" ht="18.75" customHeight="1" thickTop="1">
-      <c r="B25" s="37"/>
-      <c r="C25" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="E25" s="20"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="18"/>
+    </row>
+    <row r="21" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B21" s="32"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="18"/>
+    </row>
+    <row r="22" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B22" s="32"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="18"/>
+    </row>
+    <row r="23" spans="2:5" ht="3.75" customHeight="1">
+      <c r="B23" s="19"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="13"/>
+    </row>
+    <row r="25" spans="2:5" ht="18.75" customHeight="1">
+      <c r="E25" s="16"/>
     </row>
     <row r="26" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B26" s="37"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E26" s="17"/>
-    </row>
-    <row r="27" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B27" s="37"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="E27" s="24"/>
-    </row>
-    <row r="28" spans="2:5" ht="18.75" customHeight="1">
-      <c r="B28" s="37"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28" s="26"/>
-    </row>
-    <row r="29" spans="2:5" ht="3.75" customHeight="1">
-      <c r="B29" s="27"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="15"/>
-    </row>
-    <row r="30" spans="2:5" ht="26.25" customHeight="1">
-      <c r="B30" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="43" t="s">
-        <v>28</v>
-      </c>
-      <c r="D30" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="E30" s="30"/>
-    </row>
-    <row r="31" spans="2:5" ht="26.25" customHeight="1" thickBot="1">
-      <c r="B31" s="41"/>
-      <c r="C31" s="44"/>
-      <c r="D31" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="E31" s="32"/>
-    </row>
-    <row r="32" spans="2:5" ht="56.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B32" s="42"/>
-      <c r="C32" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="D32" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="E32" s="35"/>
-    </row>
-    <row r="33" spans="5:5" ht="18.75" customHeight="1" thickTop="1"/>
-    <row r="34" spans="5:5" ht="18.75" customHeight="1">
-      <c r="E34" s="36"/>
-    </row>
-    <row r="35" spans="5:5" ht="18.75" customHeight="1">
-      <c r="E35" s="36"/>
+      <c r="E26" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="C30:C31"/>
+  <mergeCells count="7">
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B5:B17"/>
+    <mergeCell ref="B5:B15"/>
     <mergeCell ref="C5:C7"/>
-    <mergeCell ref="C9:C14"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="B19:B28"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="C25:C28"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="B17:B22"/>
+    <mergeCell ref="C17:C22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2:E2" r:id="rId1" display="The Flatiron School Prework"/>

</xml_diff>